<commit_message>
Update Monitoramento atividades OBM_Março.xlsx
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Monitoramento/03 - Março/Monitoramento atividades OBM_Março.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Monitoramento/03 - Março/Monitoramento atividades OBM_Março.xlsx
@@ -413,6 +413,20 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,20 +460,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1927,7 +1927,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4058,7 +4057,7 @@
   <dimension ref="A3:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4080,18 +4079,18 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44" t="s">
+      <c r="F4" s="51"/>
+      <c r="G4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="44"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="26" t="s">
         <v>4</v>
       </c>
@@ -4164,13 +4163,21 @@
       <c r="B7" s="32">
         <v>14</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="27">
+        <v>1</v>
+      </c>
       <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="E7" s="28">
+        <v>15</v>
+      </c>
       <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="G7" s="29">
+        <v>15</v>
+      </c>
       <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="30">
+        <v>15</v>
+      </c>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.3">
@@ -4222,36 +4229,36 @@
       <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="43">
         <v>18</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="43">
         <v>19</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
@@ -4334,36 +4341,36 @@
       <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="58">
+      <c r="B18" s="47">
         <v>25</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="58">
+      <c r="B19" s="47">
         <v>26</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
@@ -4470,11 +4477,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -4541,10 +4548,10 @@
       <c r="C12" s="13"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="60">
+      <c r="C14" s="49">
         <v>1</v>
       </c>
     </row>
@@ -4576,12 +4583,12 @@
       </c>
     </row>
     <row r="4" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="48"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="7:17" x14ac:dyDescent="0.3">
       <c r="N5" s="15"/>
@@ -4631,10 +4638,10 @@
       <c r="Q10" s="18"/>
     </row>
     <row r="11" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="P11" s="49" t="s">
+      <c r="P11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="50"/>
+      <c r="Q11" s="58"/>
     </row>
     <row r="12" spans="7:17" x14ac:dyDescent="0.3">
       <c r="P12" s="22">
@@ -4647,17 +4654,17 @@
       </c>
     </row>
     <row r="13" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="P13" s="49" t="s">
+      <c r="P13" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="Q13" s="50"/>
+      <c r="Q13" s="58"/>
     </row>
     <row r="14" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="P14" s="51">
+      <c r="P14" s="59">
         <f>P12+Q12</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="52"/>
+      <c r="Q14" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>